<commit_message>
Trying to update data
</commit_message>
<xml_diff>
--- a/Data/admin_data.xlsx
+++ b/Data/admin_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alia/Documents/Github/LIHEAPadminapp/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314459AC-C7B3-6949-987D-60B54FE93FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0E27A72-90A8-0B49-BEC0-62C271896EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>